<commit_message>
highlight in 2020 T4 & T5 add a total plot
</commit_message>
<xml_diff>
--- a/Data_2020/Excel_files_2020/Table 4/Table_4_Offenses_Offense_Type_by_Bias_Motivation_2020.xlsx
+++ b/Data_2020/Excel_files_2020/Table 4/Table_4_Offenses_Offense_Type_by_Bias_Motivation_2020.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDCE4DA-D7CE-4A78-93BC-67AAA395AABD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EE193A-30ED-294D-A393-0A9270454AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="570" windowWidth="28725" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13680" yWindow="580" windowWidth="15120" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 4" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,6 +487,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF0F4FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -575,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -610,7 +616,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -620,7 +626,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -641,10 +647,9 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -657,6 +662,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -999,21 +1016,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C26" zoomScale="183" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="15" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="15" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="15" customWidth="1"/>
-    <col min="8" max="13" width="7.7109375" style="15" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="15" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" style="15" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="15" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="15" customWidth="1"/>
+    <col min="8" max="13" width="7.6640625" style="15" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" style="15" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="15" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1036,40 +1055,40 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="30" t="s">
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
       <c r="P6" s="18"/>
     </row>
-    <row r="7" spans="1:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="38" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="20" t="s">
         <v>51</v>
       </c>
@@ -1113,7 +1132,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1182,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
@@ -1213,7 +1232,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>35</v>
       </c>
@@ -1263,7 +1282,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>8</v>
       </c>
@@ -1313,7 +1332,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>9</v>
       </c>
@@ -1363,7 +1382,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>10</v>
       </c>
@@ -1413,7 +1432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>11</v>
       </c>
@@ -1463,7 +1482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>12</v>
       </c>
@@ -1513,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>58</v>
       </c>
@@ -1563,7 +1582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>13</v>
       </c>
@@ -1613,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
         <v>14</v>
       </c>
@@ -1663,7 +1682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
         <v>36</v>
       </c>
@@ -1713,7 +1732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>37</v>
       </c>
@@ -1763,7 +1782,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>15</v>
       </c>
@@ -1813,7 +1832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
         <v>16</v>
       </c>
@@ -1863,7 +1882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
         <v>17</v>
       </c>
@@ -1913,7 +1932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>18</v>
       </c>
@@ -1963,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
         <v>19</v>
       </c>
@@ -2013,7 +2032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="24" t="s">
         <v>59</v>
       </c>
@@ -2063,7 +2082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
         <v>20</v>
       </c>
@@ -2113,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>21</v>
       </c>
@@ -2163,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
         <v>38</v>
       </c>
@@ -2213,7 +2232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="24" t="s">
         <v>22</v>
       </c>
@@ -2263,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
         <v>23</v>
       </c>
@@ -2313,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="24" t="s">
         <v>24</v>
       </c>
@@ -2363,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="24" t="s">
         <v>25</v>
       </c>
@@ -2413,7 +2432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="24" t="s">
         <v>62</v>
       </c>
@@ -2463,8 +2482,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="33" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="6">
@@ -2482,7 +2501,7 @@
       <c r="F35" s="6">
         <v>370</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="31">
         <v>1254</v>
       </c>
       <c r="H35" s="6">
@@ -2513,7 +2532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
         <v>40</v>
       </c>
@@ -2532,7 +2551,7 @@
       <c r="F36" s="8">
         <v>252</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="34">
         <v>203</v>
       </c>
       <c r="H36" s="8">
@@ -2563,7 +2582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="24" t="s">
         <v>41</v>
       </c>
@@ -2582,7 +2601,7 @@
       <c r="F37" s="8">
         <v>28</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="32">
         <v>940</v>
       </c>
       <c r="H37" s="10">
@@ -2613,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
         <v>42</v>
       </c>
@@ -2632,7 +2651,7 @@
       <c r="F38" s="8">
         <v>84</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="34">
         <v>102</v>
       </c>
       <c r="H38" s="10">
@@ -2663,7 +2682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="24" t="s">
         <v>26</v>
       </c>
@@ -2713,7 +2732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="24" t="s">
         <v>27</v>
       </c>
@@ -2763,7 +2782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
         <v>43</v>
       </c>
@@ -2811,7 +2830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="24" t="s">
         <v>44</v>
       </c>
@@ -2861,7 +2880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="24" t="s">
         <v>45</v>
       </c>
@@ -2911,7 +2930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
         <v>46</v>
       </c>
@@ -2959,7 +2978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="24" t="s">
         <v>28</v>
       </c>
@@ -3009,7 +3028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="24" t="s">
         <v>29</v>
       </c>
@@ -3059,7 +3078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
         <v>47</v>
       </c>
@@ -3072,13 +3091,13 @@
       <c r="D47" s="6">
         <v>1</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="31">
         <v>61</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="31">
         <v>90</v>
       </c>
-      <c r="G47" s="6">
+      <c r="G47" s="31">
         <v>60</v>
       </c>
       <c r="H47" s="6">
@@ -3109,7 +3128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="24" t="s">
         <v>30</v>
       </c>
@@ -3122,13 +3141,13 @@
       <c r="D48" s="10">
         <v>0</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48" s="32">
         <v>57</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F48" s="32">
         <v>76</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="32">
         <v>52</v>
       </c>
       <c r="H48" s="8">
@@ -3159,7 +3178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
         <v>31</v>
       </c>
@@ -3209,7 +3228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
         <v>66</v>
       </c>
@@ -3259,7 +3278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="25" t="s">
         <v>67</v>
       </c>
@@ -3272,14 +3291,14 @@
       <c r="H51" s="25"/>
       <c r="I51" s="25"/>
       <c r="J51" s="26"/>
-      <c r="K51" s="27"/>
-      <c r="L51" s="27"/>
-      <c r="M51" s="27"/>
-      <c r="N51" s="27"/>
-      <c r="O51" s="27"/>
-      <c r="P51" s="27"/>
-    </row>
-    <row r="52" spans="1:16" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
+      <c r="P51" s="26"/>
+    </row>
+    <row r="52" spans="1:16" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>61</v>
       </c>
@@ -3299,7 +3318,7 @@
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
     </row>
-    <row r="53" spans="1:16" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>60</v>
       </c>

</xml_diff>